<commit_message>
Fixed accidental upload of ImmGen .csv file, plus analysis scripts for ImmGen data
</commit_message>
<xml_diff>
--- a/ifnscripts/NIH/ImmGen_signaling_with_protein_response.xlsx
+++ b/ifnscripts/NIH/ImmGen_signaling_with_protein_response.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan\Documents\University\Grad Studies Year 3\IFNmodeling\ifnscripts\NIH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DA78C2-E71B-46B9-B8B0-D59288839F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25801F52-6298-4638-9576-BAB71DE05E1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="2928" windowWidth="17280" windowHeight="8964" xr2:uid="{BE3BC1B7-7AF4-E24A-A9FC-0EA6487230DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BE3BC1B7-7AF4-E24A-A9FC-0EA6487230DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>pSTAT1</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Cell_type</t>
+  </si>
+  <si>
+    <t>USP18</t>
   </si>
 </sst>
 </file>
@@ -514,15 +517,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4700B123-ADBB-9546-81E9-2D17A79F6628}">
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -598,8 +601,11 @@
       <c r="Y1" t="s">
         <v>35</v>
       </c>
+      <c r="Z1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -675,8 +681,11 @@
       <c r="Y2">
         <v>2240.0500000000002</v>
       </c>
+      <c r="Z2">
+        <v>308.851</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -752,8 +761,11 @@
       <c r="Y3">
         <v>1927.14</v>
       </c>
+      <c r="Z3">
+        <v>299.661</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -829,8 +841,11 @@
       <c r="Y4">
         <v>1780.07</v>
       </c>
+      <c r="Z4">
+        <v>115.9</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -906,8 +921,11 @@
       <c r="Y5">
         <v>532.10299999999995</v>
       </c>
+      <c r="Z5">
+        <v>90.226699999999994</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -983,8 +1001,11 @@
       <c r="Y6">
         <v>960.38699999999994</v>
       </c>
+      <c r="Z6">
+        <v>120.015</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1060,8 +1081,11 @@
       <c r="Y7">
         <v>394.09800000000001</v>
       </c>
+      <c r="Z7">
+        <v>207.27</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1137,8 +1161,11 @@
       <c r="Y8">
         <v>346.36700000000002</v>
       </c>
+      <c r="Z8">
+        <v>179.98099999999999</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1214,8 +1241,11 @@
       <c r="Y9">
         <v>276.44900000000001</v>
       </c>
+      <c r="Z9">
+        <v>178.26</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1291,8 +1321,11 @@
       <c r="Y10">
         <v>573.08600000000001</v>
       </c>
+      <c r="Z10">
+        <v>78.415899999999993</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1368,8 +1401,11 @@
       <c r="Y11">
         <v>285.34100000000001</v>
       </c>
+      <c r="Z11">
+        <v>132.33500000000001</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1445,8 +1481,11 @@
       <c r="Y12">
         <v>1231.54</v>
       </c>
+      <c r="Z12">
+        <v>167.41499999999999</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1522,8 +1561,11 @@
       <c r="Y13">
         <v>918.78499999999997</v>
       </c>
+      <c r="Z13">
+        <v>74.055000000000007</v>
+      </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1599,8 +1641,11 @@
       <c r="Y14">
         <v>291.88600000000002</v>
       </c>
+      <c r="Z14">
+        <v>146.10499999999999</v>
+      </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1676,8 +1721,11 @@
       <c r="Y15">
         <v>489.11599999999999</v>
       </c>
+      <c r="Z15">
+        <v>152.44300000000001</v>
+      </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1753,8 +1801,11 @@
       <c r="Y16">
         <v>1228.55</v>
       </c>
+      <c r="Z16">
+        <v>147.38200000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1830,8 +1881,11 @@
       <c r="Y17">
         <v>1307.0899999999999</v>
       </c>
+      <c r="Z17">
+        <v>223.25200000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1907,8 +1961,11 @@
       <c r="Y18">
         <v>1137.6400000000001</v>
       </c>
+      <c r="Z18">
+        <v>255.25299999999999</v>
+      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1984,8 +2041,11 @@
       <c r="Y19">
         <v>87.473799999999997</v>
       </c>
+      <c r="Z19">
+        <v>126.11199999999999</v>
+      </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2060,6 +2120,9 @@
       </c>
       <c r="Y20">
         <v>625.57500000000005</v>
+      </c>
+      <c r="Z20">
+        <v>136.66999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>